<commit_message>
updated change analyses and figures
</commit_message>
<xml_diff>
--- a/data/protein/western.quant.xlsx
+++ b/data/protein/western.quant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kristili\R\ribose-paper\data\protein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F8B4DA-588F-4FA1-ACE3-A5D8A21DA10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A1D813-62CC-4914-9A47-C53285B6FC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FAEAA96B-A5E5-4AF0-AE5A-BF52CEB7DD8D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAEAA96B-A5E5-4AF0-AE5A-BF52CEB7DD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="82">
   <si>
     <t>gel</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>tot.prot</t>
   </si>
 </sst>
 </file>
@@ -639,19 +642,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E27BD1-C824-4623-B0AE-633ACA3A0674}">
-  <dimension ref="A1:S126"/>
+  <dimension ref="A1:U126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
+      <selection activeCell="U121" sqref="U121:U124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -709,8 +712,11 @@
       <c r="S1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -768,8 +774,11 @@
       <c r="S2">
         <v>12900000</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T2">
+        <v>11.5021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -827,8 +836,11 @@
       <c r="S3">
         <v>12300000</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T3">
+        <v>16.277200000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -886,8 +898,11 @@
       <c r="S4">
         <v>35100000</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T4">
+        <v>13.8453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -945,8 +960,11 @@
       <c r="S5">
         <v>22400000</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T5">
+        <v>7.5820999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -996,7 +1014,7 @@
         <v>18300000</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1054,8 +1072,11 @@
       <c r="S7">
         <v>35800000</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T7">
+        <v>16.605499999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1113,8 +1134,11 @@
       <c r="S8">
         <v>30300000</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T8">
+        <v>17.893000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1172,8 +1196,11 @@
       <c r="S9">
         <v>15300000</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T9">
+        <v>9.8752999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1231,8 +1258,11 @@
       <c r="S10">
         <v>16700000</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T10">
+        <v>11.0624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1290,8 +1320,11 @@
       <c r="S11">
         <v>15300000</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T11">
+        <v>17.706900000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1341,7 +1374,7 @@
         <v>22100000</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1399,8 +1432,11 @@
       <c r="S13">
         <v>17800000</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T13">
+        <v>7.4519000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1458,8 +1494,11 @@
       <c r="S14">
         <v>31500000</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T14">
+        <v>10.42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1517,8 +1556,11 @@
       <c r="S15">
         <v>39000000</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T15">
+        <v>14.1081</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1576,8 +1618,11 @@
       <c r="S16">
         <v>37600000</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T16">
+        <v>5.9157999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1635,8 +1680,11 @@
       <c r="S17">
         <v>22600000</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T17">
+        <v>7.9409999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1694,8 +1742,11 @@
       <c r="S18">
         <v>34600000</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T18">
+        <v>6.5709</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1753,8 +1804,11 @@
       <c r="S19">
         <v>32600000</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T19">
+        <v>4.5896999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1804,7 +1858,7 @@
         <v>25300000</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1862,8 +1916,11 @@
       <c r="S21">
         <v>11100000</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T21">
+        <v>6.8564999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1921,8 +1978,11 @@
       <c r="S22">
         <v>18900000</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T22">
+        <v>5.1608999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1980,8 +2040,11 @@
       <c r="S23">
         <v>22800000</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T23">
+        <v>5.7210000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2039,8 +2102,11 @@
       <c r="S24">
         <v>18600000</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T24">
+        <v>8.6717999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2098,8 +2164,11 @@
       <c r="S25">
         <v>16800000</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T25">
+        <v>7.5750000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2157,8 +2226,11 @@
       <c r="S26">
         <v>12900000</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T26">
+        <v>8.5182000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2216,8 +2288,11 @@
       <c r="S27">
         <v>20600000</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T27">
+        <v>4.6745000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2275,8 +2350,11 @@
       <c r="S28">
         <v>18000000</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T28">
+        <v>6.0864000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2326,7 +2404,7 @@
         <v>18500000</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2384,8 +2462,11 @@
       <c r="S30">
         <v>15900000</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T30">
+        <v>6.8334000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -2443,8 +2524,11 @@
       <c r="S31">
         <v>14400000</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T31">
+        <v>11.1694</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -2502,8 +2586,11 @@
       <c r="S32">
         <v>36000000</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T32">
+        <v>12.156599999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2561,8 +2648,11 @@
       <c r="S33">
         <v>14900000</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T33">
+        <v>9.5124999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2612,7 +2702,7 @@
         <v>17100000</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2670,8 +2760,11 @@
       <c r="S35">
         <v>14200000</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T35">
+        <v>10.065300000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -2729,8 +2822,11 @@
       <c r="S36">
         <v>24100000</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T36">
+        <v>9.0355000000000008</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -2788,8 +2884,11 @@
       <c r="S37">
         <v>24000000</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T37">
+        <v>6.0128000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -2847,8 +2946,11 @@
       <c r="S38">
         <v>16100000</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T38">
+        <v>4.6557000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2906,8 +3008,11 @@
       <c r="S39">
         <v>9530000</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T39">
+        <v>6.9226999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -2965,8 +3070,11 @@
       <c r="S40">
         <v>11600000</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T40">
+        <v>7.3975999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -3024,8 +3132,11 @@
       <c r="S41">
         <v>17600000</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T41">
+        <v>5.3219000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -3075,7 +3186,7 @@
         <v>18700000</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -3133,8 +3244,11 @@
       <c r="S43">
         <v>16200000</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T43">
+        <v>8.0067000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -3192,8 +3306,11 @@
       <c r="S44">
         <v>18900000</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T44">
+        <v>5.1547999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -3251,8 +3368,11 @@
       <c r="S45">
         <v>25900000</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T45">
+        <v>5.4824000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -3310,8 +3430,11 @@
       <c r="S46">
         <v>34600000</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T46">
+        <v>5.7061000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -3369,8 +3492,11 @@
       <c r="S47">
         <v>17900000</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T47">
+        <v>5.3526999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -3420,7 +3546,7 @@
         <v>19800000</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -3470,7 +3596,7 @@
         <v>15800000</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -3528,8 +3654,11 @@
       <c r="S50">
         <v>15800000</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T50">
+        <v>8.5611999999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -3587,8 +3716,11 @@
       <c r="S51">
         <v>20400000</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T51">
+        <v>7.1992000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -3646,8 +3778,11 @@
       <c r="S52">
         <v>21200000</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T52">
+        <v>9.0961999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
@@ -3705,8 +3840,11 @@
       <c r="S53">
         <v>23100000</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T53">
+        <v>8.7715999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -3756,7 +3894,7 @@
         <v>17900000</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -3814,8 +3952,11 @@
       <c r="S55">
         <v>32800000</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T55">
+        <v>6.5338000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3873,8 +4014,11 @@
       <c r="S56">
         <v>24500000</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T56">
+        <v>6.3338000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -3932,8 +4076,11 @@
       <c r="S57">
         <v>16700000</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T57">
+        <v>5.2206000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
@@ -3991,8 +4138,11 @@
       <c r="S58">
         <v>22300000</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T58">
+        <v>5.6836000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3</v>
       </c>
@@ -4050,8 +4200,11 @@
       <c r="S59">
         <v>29500000</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T59">
+        <v>5.8544</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -4101,7 +4254,7 @@
         <v>24300000</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -4159,8 +4312,11 @@
       <c r="S61">
         <v>17900000</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T61">
+        <v>5.0522</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -4218,8 +4374,11 @@
       <c r="S62">
         <v>22300000</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T62">
+        <v>6.0336999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3</v>
       </c>
@@ -4277,8 +4436,11 @@
       <c r="S63">
         <v>29000000</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T63">
+        <v>4.0989000000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4</v>
       </c>
@@ -4328,7 +4490,7 @@
         <v>18600000</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4</v>
       </c>
@@ -4386,8 +4548,12 @@
       <c r="S65">
         <v>16500000</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T65">
+        <v>8.6717999999999993</v>
+      </c>
+      <c r="U65" s="1"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4</v>
       </c>
@@ -4445,8 +4611,12 @@
       <c r="S66">
         <v>21500000</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T66">
+        <v>5.7210000000000001</v>
+      </c>
+      <c r="U66" s="1"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>4</v>
       </c>
@@ -4504,8 +4674,12 @@
       <c r="S67">
         <v>16900000</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T67">
+        <v>5.1608999999999998</v>
+      </c>
+      <c r="U67" s="1"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4</v>
       </c>
@@ -4563,8 +4737,12 @@
       <c r="S68">
         <v>8720000</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T68">
+        <v>6.8564999999999996</v>
+      </c>
+      <c r="U68" s="1"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4</v>
       </c>
@@ -4614,7 +4792,7 @@
         <v>17300000</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>4</v>
       </c>
@@ -4672,8 +4850,12 @@
       <c r="S70">
         <v>21800000</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T70">
+        <v>4.5896999999999997</v>
+      </c>
+      <c r="U70" s="1"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>4</v>
       </c>
@@ -4731,8 +4913,12 @@
       <c r="S71">
         <v>23900000</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T71">
+        <v>6.5709</v>
+      </c>
+      <c r="U71" s="1"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>4</v>
       </c>
@@ -4790,8 +4976,12 @@
       <c r="S72">
         <v>17300000</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T72">
+        <v>7.9409999999999998</v>
+      </c>
+      <c r="U72" s="1"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>4</v>
       </c>
@@ -4849,8 +5039,12 @@
       <c r="S73">
         <v>28500000</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T73">
+        <v>5.9157999999999999</v>
+      </c>
+      <c r="U73" s="1"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>4</v>
       </c>
@@ -4908,8 +5102,11 @@
       <c r="S74">
         <v>35000000</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T74">
+        <v>14.1081</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4</v>
       </c>
@@ -4967,8 +5164,12 @@
       <c r="S75">
         <v>27200000</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T75">
+        <v>10.42</v>
+      </c>
+      <c r="U75" s="1"/>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4</v>
       </c>
@@ -5026,8 +5227,12 @@
       <c r="S76">
         <v>15300000</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T76">
+        <v>7.4519000000000002</v>
+      </c>
+      <c r="U76" s="1"/>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4</v>
       </c>
@@ -5076,8 +5281,9 @@
       <c r="S77">
         <v>20400000</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U77" s="1"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4</v>
       </c>
@@ -5135,8 +5341,12 @@
       <c r="S78">
         <v>11300000</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T78">
+        <v>17.706900000000001</v>
+      </c>
+      <c r="U78" s="1"/>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>4</v>
       </c>
@@ -5194,8 +5404,12 @@
       <c r="S79">
         <v>13800000</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T79">
+        <v>11.0624</v>
+      </c>
+      <c r="U79" s="1"/>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>4</v>
       </c>
@@ -5253,8 +5467,12 @@
       <c r="S80">
         <v>15100000</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T80">
+        <v>9.8752999999999993</v>
+      </c>
+      <c r="U80" s="1"/>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4</v>
       </c>
@@ -5312,8 +5530,12 @@
       <c r="S81">
         <v>28200000</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T81">
+        <v>17.893000000000001</v>
+      </c>
+      <c r="U81" s="1"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4</v>
       </c>
@@ -5371,8 +5593,12 @@
       <c r="S82">
         <v>30400000</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T82">
+        <v>16.605499999999999</v>
+      </c>
+      <c r="U82" s="1"/>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>4</v>
       </c>
@@ -5422,7 +5648,7 @@
         <v>18600000</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>4</v>
       </c>
@@ -5480,8 +5706,12 @@
       <c r="S84">
         <v>23800000</v>
       </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T84">
+        <v>7.5820999999999996</v>
+      </c>
+      <c r="U84" s="1"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4</v>
       </c>
@@ -5539,8 +5769,12 @@
       <c r="S85">
         <v>33400000</v>
       </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T85">
+        <v>13.8453</v>
+      </c>
+      <c r="U85" s="1"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4</v>
       </c>
@@ -5598,8 +5832,12 @@
       <c r="S86">
         <v>13100000</v>
       </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T86">
+        <v>16.277200000000001</v>
+      </c>
+      <c r="U86" s="1"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>4</v>
       </c>
@@ -5657,8 +5895,12 @@
       <c r="S87">
         <v>14900000</v>
       </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T87">
+        <v>11.5021</v>
+      </c>
+      <c r="U87" s="1"/>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5</v>
       </c>
@@ -5708,7 +5950,7 @@
         <v>22700000</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5</v>
       </c>
@@ -5766,8 +6008,12 @@
       <c r="S89">
         <v>19400000</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T89">
+        <v>5.3526999999999996</v>
+      </c>
+      <c r="U89" s="1"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5</v>
       </c>
@@ -5825,8 +6071,12 @@
       <c r="S90">
         <v>33700000</v>
       </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T90">
+        <v>5.7061000000000002</v>
+      </c>
+      <c r="U90" s="1"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5</v>
       </c>
@@ -5884,8 +6134,12 @@
       <c r="S91">
         <v>27000000</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T91">
+        <v>5.4824000000000002</v>
+      </c>
+      <c r="U91" s="1"/>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>5</v>
       </c>
@@ -5943,8 +6197,12 @@
       <c r="S92">
         <v>22400000</v>
       </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T92">
+        <v>5.1547999999999998</v>
+      </c>
+      <c r="U92" s="1"/>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5</v>
       </c>
@@ -6002,8 +6260,12 @@
       <c r="S93">
         <v>21900000</v>
       </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T93">
+        <v>8.0067000000000004</v>
+      </c>
+      <c r="U93" s="1"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5</v>
       </c>
@@ -6052,8 +6314,9 @@
       <c r="S94">
         <v>22300000</v>
       </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U94" s="1"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5</v>
       </c>
@@ -6111,8 +6374,12 @@
       <c r="S95">
         <v>21100000</v>
       </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T95">
+        <v>5.3219000000000003</v>
+      </c>
+      <c r="U95" s="1"/>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5</v>
       </c>
@@ -6170,8 +6437,12 @@
       <c r="S96">
         <v>16200000</v>
       </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T96">
+        <v>7.3975999999999997</v>
+      </c>
+      <c r="U96" s="1"/>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>5</v>
       </c>
@@ -6229,8 +6500,11 @@
       <c r="S97">
         <v>13800000</v>
       </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T97">
+        <v>6.9226999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5</v>
       </c>
@@ -6288,8 +6562,11 @@
       <c r="S98">
         <v>18900000</v>
       </c>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T98">
+        <v>4.6557000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5</v>
       </c>
@@ -6347,8 +6624,12 @@
       <c r="S99">
         <v>27800000</v>
       </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T99">
+        <v>6.0128000000000004</v>
+      </c>
+      <c r="U99" s="1"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5</v>
       </c>
@@ -6406,8 +6687,12 @@
       <c r="S100">
         <v>27900000</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T100">
+        <v>9.0355000000000008</v>
+      </c>
+      <c r="U100" s="1"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5</v>
       </c>
@@ -6465,8 +6750,12 @@
       <c r="S101">
         <v>18300000</v>
       </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T101">
+        <v>10.065300000000001</v>
+      </c>
+      <c r="U101" s="1"/>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5</v>
       </c>
@@ -6515,8 +6804,9 @@
       <c r="S102">
         <v>19700000</v>
       </c>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U102" s="1"/>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>5</v>
       </c>
@@ -6574,8 +6864,12 @@
       <c r="S103">
         <v>15100000</v>
       </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T103">
+        <v>9.5124999999999993</v>
+      </c>
+      <c r="U103" s="1"/>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>5</v>
       </c>
@@ -6633,8 +6927,12 @@
       <c r="S104">
         <v>32700000</v>
       </c>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T104">
+        <v>12.156599999999999</v>
+      </c>
+      <c r="U104" s="1"/>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>5</v>
       </c>
@@ -6692,8 +6990,12 @@
       <c r="S105">
         <v>11900000</v>
       </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T105">
+        <v>11.1694</v>
+      </c>
+      <c r="U105" s="1"/>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>5</v>
       </c>
@@ -6751,8 +7053,11 @@
       <c r="S106">
         <v>18200000</v>
       </c>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T106">
+        <v>6.8334000000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>5</v>
       </c>
@@ -6801,8 +7106,9 @@
       <c r="S107">
         <v>18700000</v>
       </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U107" s="1"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>5</v>
       </c>
@@ -6860,8 +7166,12 @@
       <c r="S108">
         <v>20300000</v>
       </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T108">
+        <v>6.0864000000000003</v>
+      </c>
+      <c r="U108" s="1"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>5</v>
       </c>
@@ -6919,8 +7229,12 @@
       <c r="S109">
         <v>22800000</v>
       </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T109">
+        <v>4.6745000000000001</v>
+      </c>
+      <c r="U109" s="1"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>5</v>
       </c>
@@ -6978,8 +7292,12 @@
       <c r="S110">
         <v>15200000</v>
       </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T110">
+        <v>8.5182000000000002</v>
+      </c>
+      <c r="U110" s="1"/>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>5</v>
       </c>
@@ -7037,8 +7355,11 @@
       <c r="S111">
         <v>21600000</v>
       </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T111">
+        <v>7.5750000000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>6</v>
       </c>
@@ -7096,8 +7417,12 @@
       <c r="S112">
         <v>24900000</v>
       </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T112">
+        <v>4.0989000000000004</v>
+      </c>
+      <c r="U112" s="1"/>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>6</v>
       </c>
@@ -7155,8 +7480,12 @@
       <c r="S113">
         <v>16600000</v>
       </c>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T113">
+        <v>6.0336999999999996</v>
+      </c>
+      <c r="U113" s="1"/>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>6</v>
       </c>
@@ -7214,8 +7543,12 @@
       <c r="S114">
         <v>11400000</v>
       </c>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T114">
+        <v>5.0522</v>
+      </c>
+      <c r="U114" s="1"/>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>6</v>
       </c>
@@ -7264,8 +7597,9 @@
       <c r="S115">
         <v>15800000</v>
       </c>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U115" s="1"/>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>6</v>
       </c>
@@ -7323,8 +7657,11 @@
       <c r="S116">
         <v>19300000</v>
       </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T116">
+        <v>5.8544</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>6</v>
       </c>
@@ -7382,8 +7719,12 @@
       <c r="S117">
         <v>17600000</v>
       </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T117">
+        <v>5.6836000000000002</v>
+      </c>
+      <c r="U117" s="1"/>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>6</v>
       </c>
@@ -7441,8 +7782,12 @@
       <c r="S118">
         <v>17000000</v>
       </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T118">
+        <v>5.2206000000000001</v>
+      </c>
+      <c r="U118" s="1"/>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>6</v>
       </c>
@@ -7500,8 +7845,12 @@
       <c r="S119">
         <v>31100000</v>
       </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T119">
+        <v>6.3338000000000001</v>
+      </c>
+      <c r="U119" s="1"/>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>6</v>
       </c>
@@ -7559,8 +7908,12 @@
       <c r="S120">
         <v>40700000</v>
       </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T120">
+        <v>6.5338000000000003</v>
+      </c>
+      <c r="U120" s="1"/>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>6</v>
       </c>
@@ -7609,8 +7962,9 @@
       <c r="S121">
         <v>26000000</v>
       </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U121" s="1"/>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>6</v>
       </c>
@@ -7668,8 +8022,12 @@
       <c r="S122">
         <v>31900000</v>
       </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T122">
+        <v>8.7715999999999994</v>
+      </c>
+      <c r="U122" s="1"/>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>6</v>
       </c>
@@ -7727,8 +8085,12 @@
       <c r="S123">
         <v>25400000</v>
       </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T123">
+        <v>9.0961999999999996</v>
+      </c>
+      <c r="U123" s="1"/>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>6</v>
       </c>
@@ -7786,8 +8148,12 @@
       <c r="S124">
         <v>25600000</v>
       </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T124">
+        <v>7.1992000000000003</v>
+      </c>
+      <c r="U124" s="1"/>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>6</v>
       </c>
@@ -7845,8 +8211,11 @@
       <c r="S125">
         <v>18600000</v>
       </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T125">
+        <v>8.5611999999999995</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>6</v>
       </c>

</xml_diff>